<commit_message>
DDT framework update and grouping
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaRefresh2024\demo17122025\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26B1E68-2989-40B8-B0EA-BAC6B3A4CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58658DB3-C519-4CC6-AAE1-46DC04514E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="17280" windowHeight="8880" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -60,23 +60,20 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>abc123@gmail.com</t>
-  </si>
-  <si>
     <t>ce.hardikdave@gmail.com</t>
   </si>
   <si>
     <t>Encrypt@1827</t>
+  </si>
+  <si>
+    <t>ce.hardikrdave@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,14 +92,6 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="16"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,18 +139,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -484,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884FCF78-0A3E-40BF-9E26-11C478AF56E2}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -507,58 +490,58 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>5</v>
+      <c r="C6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -567,8 +550,8 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{5E52A498-5B14-4BDC-BBF1-05425B8AC197}"/>
     <hyperlink ref="A5" r:id="rId3" xr:uid="{94E9D5A6-98A1-4A25-BDDE-C5B20EDA887E}"/>
     <hyperlink ref="A6" r:id="rId4" xr:uid="{75A4F8D6-7BF1-446B-9367-475FA4FB44C7}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{01D5649A-5E55-45E1-9B81-1CE430C208A1}"/>
-    <hyperlink ref="A2" r:id="rId6" xr:uid="{EBC0021F-2DBB-4C2D-B43A-6EEC1B3B5F9E}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{EBC0021F-2DBB-4C2D-B43A-6EEC1B3B5F9E}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{6B596B37-C97C-45E9-844A-CB751218E7C4}"/>
     <hyperlink ref="B2" r:id="rId7" xr:uid="{9D88E8CB-0202-4B08-86FB-F9476598E172}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>